<commit_message>
v4 final con colres y filas nan no aparecen
</commit_message>
<xml_diff>
--- a/dist/01_08012025.xlsx
+++ b/dist/01_08012025.xlsx
@@ -5,12 +5,12 @@
   <workbookPr updateLinks="never" codeName="현재_통합_문서" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\pyAlhambra\pyAlhambra\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\migue\Desktop\pyAlhambra\pyAlhambra\dist\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8CBD3FFA-3607-4CAE-BD67-A8B01891B6FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{316A33D5-B975-48A1-AB5B-5DEF863A11A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38304" yWindow="3852" windowWidth="14592" windowHeight="15576" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38292" yWindow="3744" windowWidth="29016" windowHeight="15696" tabRatio="775" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="루밍" sheetId="25" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="289">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1076" uniqueCount="288">
   <si>
     <t>상품명</t>
   </si>
@@ -985,9 +985,6 @@
   </si>
   <si>
     <t>GUIA COREANO</t>
-  </si>
-  <si>
-    <t>LIM KYUNG RAN1</t>
   </si>
 </sst>
 </file>
@@ -1937,7 +1934,7 @@
   <dimension ref="A1:BB48"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10" defaultRowHeight="14.4"/>
@@ -2125,7 +2122,7 @@
         <v>38</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>288</v>
+        <v>39</v>
       </c>
       <c r="E6" s="11" t="s">
         <v>6</v>
@@ -2137,37 +2134,37 @@
         <v>187</v>
       </c>
       <c r="H6" s="13"/>
-      <c r="I6" s="33" t="e">
+      <c r="I6" s="33" t="str">
         <f t="shared" ref="I6:I47" si="0">INDEX($V$6:$V$500,MATCH(D6,$U$6:$U$500,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="J6" s="33" t="e">
+        <v>1972-02-06</v>
+      </c>
+      <c r="J6" s="33" t="str">
         <f t="shared" ref="J6:J47" si="1">INDEX($Y$6:$Y$500,MATCH($D6,$U$6:$U$500,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="K6" s="33" t="e">
+        <v>M719M6705</v>
+      </c>
+      <c r="K6" s="33" t="str">
         <f t="shared" ref="K6:K47" si="2">INDEX($Z$6:$Z$500,MATCH($D6,$U$6:$U$500,0))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="L6" s="34" t="e">
+        <v>2032-11-08</v>
+      </c>
+      <c r="L6" s="34" t="str">
         <f t="shared" ref="L6:L47" si="3">CLEAN(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(SUBSTITUTE(INDEX($AV$6:$AV$500,MATCH(D6,$AM$6:$AM$500,0)),"선택관광 : ",""),"마드리드 연장투어(달달한 추로스 포함)(EUR)50.00","MAD연장(50)"),"플라멩코[Flamenco] 공연(EUR)","플라멩고"),"그라나다 연장 투어(EUR)","GRX연장"),"몬세라트 수도원 (편도 케이블카 포함)(EUR)","몬세랏옵션"),"몬주익 언덕 투어(몬주익 성 내부 및 케이블카 포함)(EUR)50.00","몬주익(50)"),"바르셀로나 연장투어(EUR)50.00","BCN연장(50)"),"객실1인사용료 : (KRW)","싱글"),"센딩 : 일반센딩(KRW)0(OK)",""),"여행자보험 : (KRW)0(OK)",""),"제세공과금 : (KRW)0(OK)",""),"유류할증료 : (KRW)232,400(OK)",""),"유류할증료 : (KRW)207,200(OK)",""),"유류할증료 : (KRW)0(OK)",""),"유류할증료 : (KRW)680,000(OK)",""),"유류할증료 : (KRW)600,000(OK)",""),"유류할증료 : (KRW)122,800(OK)","")," [하나팩2.0] 포르투 연장투어(EUR)50.00","OPO연장50"),"일차 ","#"),"팁 : (EUR)","팁"),"(WT)","/"))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="M6" s="35" t="e">
+        <v/>
+      </c>
+      <c r="M6" s="35" t="str">
         <f>CLEAN(INDEX($AW$6:$AW$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="N6" s="35" t="e">
+        <v/>
+      </c>
+      <c r="N6" s="35" t="str">
         <f>CLEAN(INDEX($AX$6:$AX$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="O6" s="35" t="e">
+        <v/>
+      </c>
+      <c r="O6" s="35" t="str">
         <f>CLEAN(INDEX($AY$6:$AY$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v>#N/A</v>
-      </c>
-      <c r="P6" s="35" t="e">
+        <v/>
+      </c>
+      <c r="P6" s="35" t="str">
         <f>CLEAN(INDEX($AZ$6:$AZ$500,MATCH(D6,$AM$6:$AM$500,0)))</f>
-        <v>#N/A</v>
+        <v/>
       </c>
       <c r="Q6" s="30" t="s">
         <v>19</v>

</xml_diff>